<commit_message>
Improved ISA documentation, added rst line to regs.
</commit_message>
<xml_diff>
--- a/Excel/ISA Documentation.xlsx
+++ b/Excel/ISA Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\riscVcoreAutomation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98BBADEB-F020-4C46-8225-5D95FF18B139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CFE042-4AC6-4D65-9715-D8B9E6B7E0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>RISC CORE ISA</t>
   </si>
@@ -53,9 +53,6 @@
     <t>RB</t>
   </si>
   <si>
-    <t>WA</t>
-  </si>
-  <si>
     <t>DATA</t>
   </si>
   <si>
@@ -168,6 +165,123 @@
   </si>
   <si>
     <t>x(RA + DATA) = RB</t>
+  </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>ADD 3 = R1+R2</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0010</t>
+  </si>
+  <si>
+    <t>0011</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>0000_0001_0010_0011_00000000</t>
+  </si>
+  <si>
+    <t>1011_0000_0011_0000_00000011</t>
+  </si>
+  <si>
+    <t>1010_0000_0000_0001_00000000</t>
+  </si>
+  <si>
+    <t>1010_0000_0000_0010_00000001</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>1010_0000_0000_0001_00000100</t>
+  </si>
+  <si>
+    <t>load 1 = x(0+0)</t>
+  </si>
+  <si>
+    <t>load 2 = x(0+1)</t>
+  </si>
+  <si>
+    <t>STORE x(0+3) = R3</t>
+  </si>
+  <si>
+    <t>1000_0001_0000_0010_00000101</t>
+  </si>
+  <si>
+    <t>LOAD 1 = x(0+4)</t>
+  </si>
+  <si>
+    <t>ADDI R2 = R1+5</t>
+  </si>
+  <si>
+    <t>1011_0000_0010_0000_00001000</t>
+  </si>
+  <si>
+    <t>STORE x(0+8) = R2</t>
+  </si>
+  <si>
+    <t>1100_0001_0010_0000_00000010</t>
+  </si>
+  <si>
+    <t>BEQ R1==R2 +2</t>
+  </si>
+  <si>
+    <t>0001_0001_0010_0011_00000000</t>
+  </si>
+  <si>
+    <t>R3=R1-R2</t>
+  </si>
+  <si>
+    <t>1110_0000_0000_0000_00000111</t>
+  </si>
+  <si>
+    <t>JMP 7</t>
+  </si>
+  <si>
+    <t>1111_0000_0000_0000_00000000</t>
   </si>
 </sst>
 </file>
@@ -203,8 +317,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,28 +654,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3793813-9B20-438F-90FC-3E0D3543C5BE}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -571,218 +697,283 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="G13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B7:B22" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First work towards memory reading
</commit_message>
<xml_diff>
--- a/Excel/ISA Documentation.xlsx
+++ b/Excel/ISA Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\riscVcoreAutomation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thega\Projects\riscVcoreAutomation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CFE042-4AC6-4D65-9715-D8B9E6B7E0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE9D8B-21E5-4F6A-87DA-A3306507B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>if RA ~= RB then PC += DATA</t>
   </si>
   <si>
-    <t>PC = RA</t>
-  </si>
-  <si>
     <t>stop execution</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>1111_0000_0000_0000_00000000</t>
+  </si>
+  <si>
+    <t>PC = RA+DATA</t>
   </si>
 </sst>
 </file>
@@ -656,37 +656,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3793813-9B20-438F-90FC-3E0D3543C5BE}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="135" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -697,19 +697,19 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -726,21 +726,21 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
         <v>61</v>
       </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
       <c r="H5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -751,222 +751,222 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
       <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" t="s">
         <v>73</v>
       </c>
-      <c r="H9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
       <c r="G10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
         <v>75</v>
       </c>
-      <c r="H10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
       </c>
       <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s">
         <v>77</v>
       </c>
-      <c r="H11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
       </c>
       <c r="G12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" t="s">
         <v>79</v>
       </c>
-      <c r="H12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added top module, instantiated all components, need MUXing
</commit_message>
<xml_diff>
--- a/Excel/ISA Documentation.xlsx
+++ b/Excel/ISA Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thega\Projects\riscVcoreAutomation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\riscVcoreAutomation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE9D8B-21E5-4F6A-87DA-A3306507B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFE3980-54FE-4FA1-B17E-E06CF4CD8B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>RISC CORE ISA</t>
   </si>
@@ -203,21 +203,6 @@
     <t>1010</t>
   </si>
   <si>
-    <t>1011</t>
-  </si>
-  <si>
-    <t>1100</t>
-  </si>
-  <si>
-    <t>1101</t>
-  </si>
-  <si>
-    <t>1110</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
     <t>0000_0001_0010_0011_00000000</t>
   </si>
   <si>
@@ -281,7 +266,10 @@
     <t>1111_0000_0000_0000_00000000</t>
   </si>
   <si>
-    <t>PC = RA+DATA</t>
+    <t>PC = RA + DATA</t>
+  </si>
+  <si>
+    <t>(or immediate jump with R0 + DATA)</t>
   </si>
 </sst>
 </file>
@@ -654,20 +642,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3793813-9B20-438F-90FC-3E0D3543C5BE}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="135" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="135" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,18 +663,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -697,19 +685,19 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -726,246 +714,324 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
         <v>61</v>
       </c>
-      <c r="H5" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H16" t="s">
         <v>72</v>
       </c>
-      <c r="H9" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H17" t="s">
         <v>74</v>
       </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1011</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1110</v>
+      </c>
+      <c r="D26" t="s">
         <v>76</v>
       </c>
-      <c r="H11" t="s">
+      <c r="E26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B27" s="1">
+        <v>1111</v>
+      </c>
+      <c r="D27" t="s">
         <v>40</v>
       </c>
     </row>
@@ -973,7 +1039,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B7:B22" numberStoredAsText="1"/>
+    <ignoredError sqref="B12:B22" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First full sim build, working on synthesis
The cpu can now properly perform branching operations through a side datapath specifically for the program counter. branching was treated as signed, while jump was kept unsigned. My next steps will be towards learning IP for the purposes of live ROM flashes on a synthesized board.
</commit_message>
<xml_diff>
--- a/Excel/ISA Documentation.xlsx
+++ b/Excel/ISA Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\riscVcoreAutomation\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFE3980-54FE-4FA1-B17E-E06CF4CD8B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57225630-11A9-4107-9A58-50AA16AD7EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="79">
   <si>
     <t>RISC CORE ISA</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>(or immediate jump with R0 + DATA)</t>
+  </si>
+  <si>
+    <t>(signed DATA)</t>
   </si>
 </sst>
 </file>
@@ -644,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3793813-9B20-438F-90FC-3E0D3543C5BE}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="135" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,6 +1001,9 @@
       <c r="D24" t="s">
         <v>38</v>
       </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1008,6 +1014,9 @@
       </c>
       <c r="D25" t="s">
         <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
laid work for UART communication modules
</commit_message>
<xml_diff>
--- a/Excel/ISA Documentation.xlsx
+++ b/Excel/ISA Documentation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\riscVcoreAutomation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ProtoCore\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57225630-11A9-4107-9A58-50AA16AD7EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D452019B-7919-441A-BACD-1751147EE9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B12F2B8D-ADA6-4D34-B7FA-CEA8D28977FA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>RISC CORE ISA</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>(signed DATA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: </t>
+  </si>
+  <si>
+    <t>FFF000 and FFFF00 are reserved words in the CPU, and are used in the ROM_FLASHING program to signify the end of transmission of new words. As of now</t>
+  </si>
+  <si>
+    <t>these words are illegal syntax, and cannot be created regardless, but if these are somehow created and flashed in accidentally, the flash will terminate early.</t>
   </si>
 </sst>
 </file>
@@ -645,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3793813-9B20-438F-90FC-3E0D3543C5BE}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,6 +1053,19 @@
         <v>40</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>